<commit_message>
UPdate attendance list for second group
</commit_message>
<xml_diff>
--- a/lists/second-group.xlsx
+++ b/lists/second-group.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="16">
   <si>
     <t>Име</t>
   </si>
@@ -497,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,11 +509,11 @@
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" hidden="1" customWidth="1"/>
     <col min="4" max="17" width="14" hidden="1" customWidth="1"/>
-    <col min="18" max="21" width="14" customWidth="1"/>
-    <col min="22" max="1027" width="8.5703125" customWidth="1"/>
+    <col min="18" max="22" width="14" customWidth="1"/>
+    <col min="23" max="1028" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -569,16 +569,19 @@
         <v>43230</v>
       </c>
       <c r="S1" s="3">
+        <v>43230</v>
+      </c>
+      <c r="T1" s="3">
         <v>43237</v>
       </c>
-      <c r="T1" s="3">
+      <c r="U1" s="3">
         <v>43244</v>
       </c>
-      <c r="U1" s="3">
+      <c r="V1" s="3">
         <v>43251</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -634,7 +637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -680,8 +683,11 @@
       <c r="R3" t="s">
         <v>4</v>
       </c>
+      <c r="S3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -730,8 +736,11 @@
       <c r="R4" t="s">
         <v>4</v>
       </c>
+      <c r="S4" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -786,8 +795,11 @@
       <c r="R5" t="s">
         <v>14</v>
       </c>
+      <c r="S5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -839,8 +851,14 @@
       <c r="Q6" t="s">
         <v>4</v>
       </c>
+      <c r="R6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S6" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -892,8 +910,11 @@
       <c r="R7" t="s">
         <v>4</v>
       </c>
+      <c r="S7" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -948,8 +969,11 @@
       <c r="R8" t="s">
         <v>4</v>
       </c>
+      <c r="S8" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -995,8 +1019,11 @@
       <c r="R9" t="s">
         <v>4</v>
       </c>
+      <c r="S9" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>

</xml_diff>